<commit_message>
17-02-2026 Test case update by this date (Akash varun)
</commit_message>
<xml_diff>
--- a/Icaffe_Tracker.xlsx
+++ b/Icaffe_Tracker.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="101">
   <si>
     <t>MODULES</t>
   </si>
@@ -311,28 +311,46 @@
     <t>GST Invoice-&gt;Transport-&gt;Print</t>
   </si>
   <si>
+    <t>(this bug ID is used because the same issue occurs. - 630,632)</t>
+  </si>
+  <si>
+    <t>TransportInvoice_Print</t>
+  </si>
+  <si>
+    <t>GST Invoice-&gt;Transport</t>
+  </si>
+  <si>
+    <t>GST Invoice-&gt;Other Invoice</t>
+  </si>
+  <si>
+    <t>GST Invoice-&gt;Other Invoice&gt;Search</t>
+  </si>
+  <si>
+    <t>Other_Invoice</t>
+  </si>
+  <si>
+    <t>OtherInvoice_Search</t>
+  </si>
+  <si>
+    <t>GST Invoice-&gt;Other Invoice&gt;Print</t>
+  </si>
+  <si>
+    <t>OtherInvoice_Print</t>
+  </si>
+  <si>
+    <t>(this bug ID is used because the same issue occurs. - 713,719)</t>
+  </si>
+  <si>
+    <t>Hemant</t>
+  </si>
+  <si>
+    <t>GST Invoice-&gt;Consultancy Invoice</t>
+  </si>
+  <si>
     <t>Working</t>
   </si>
   <si>
-    <t>(this bug ID is used because the same issue occurs. - 630,632)</t>
-  </si>
-  <si>
-    <t>TransportInvoice_Print</t>
-  </si>
-  <si>
-    <t>GST Invoice-&gt;Transport</t>
-  </si>
-  <si>
-    <t>GST Invoice-&gt;Other Invoice</t>
-  </si>
-  <si>
-    <t>GST Invoice-&gt;Other Invoice&gt;Search</t>
-  </si>
-  <si>
-    <t>Other_Invoice</t>
-  </si>
-  <si>
-    <t>OtherInvoice_Search</t>
+    <t>Consultancy_Invoice</t>
   </si>
 </sst>
 </file>
@@ -539,7 +557,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -682,9 +700,8 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -997,12 +1014,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:S30"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,7 +1976,9 @@
         <v>45929</v>
       </c>
       <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
+      <c r="M17" s="32" t="s">
+        <v>97</v>
+      </c>
       <c r="N17" s="4" t="s">
         <v>16</v>
       </c>
@@ -2197,11 +2216,11 @@
         <v>111</v>
       </c>
       <c r="F22" s="13">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="8">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I22" s="8">
         <v>0</v>
@@ -2342,20 +2361,20 @@
         <v>35</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D25" s="6">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E25" s="6">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F25" s="6">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="6">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I25" s="6">
         <v>0</v>
@@ -2474,10 +2493,10 @@
         <v>16</v>
       </c>
       <c r="O27" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="P27" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="P27" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="Q27" s="16" t="str">
         <f>HYPERLINK("[Icaffe_Export Sea_Operaton Test Cases.xlsx]TransportInvoice_Print!A1","Go to  TransportInvoice_Print")</f>
@@ -2521,7 +2540,7 @@
       </c>
       <c r="O28" s="10"/>
       <c r="P28" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q28" s="16" t="str">
         <f>HYPERLINK("[Icaffe_Export Sea_Operaton Test Cases.xlsx]TransportInvoice_Print!A1","Go to  TransportInvoice_Print")</f>
@@ -2540,7 +2559,7 @@
         <v>35</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D29" s="18">
         <v>205</v>
@@ -2571,7 +2590,7 @@
       </c>
       <c r="O29" s="10"/>
       <c r="P29" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q29" s="16" t="str">
         <f>HYPERLINK("[Icaffe_Export Sea_Operaton Test Cases.xlsx]Other_Invoice!A1","Go to  Other_Invoice")</f>
@@ -2590,20 +2609,20 @@
         <v>35</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="6">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="E30" s="6">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F30" s="6">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I30" s="6">
         <v>0</v>
@@ -2611,19 +2630,19 @@
       <c r="J30" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K30" s="50">
+      <c r="K30" s="19">
         <v>46066</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="2" t="s">
-        <v>87</v>
+      <c r="N30" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="O30" s="2"/>
-      <c r="P30" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q30" s="51" t="str">
+      <c r="P30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q30" s="16" t="str">
         <f>HYPERLINK("[Icaffe_Export Sea_Operaton Test Cases.xlsx]OtherInvoice_Search!A1","Go to  OtherInvoice_Search")</f>
         <v>Go to  OtherInvoice_Search</v>
       </c>
@@ -2631,6 +2650,152 @@
         <v>11</v>
       </c>
       <c r="S30" s="2"/>
+    </row>
+    <row r="31" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="10">
+        <v>52</v>
+      </c>
+      <c r="E31" s="10">
+        <v>32</v>
+      </c>
+      <c r="F31" s="10">
+        <v>20</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10">
+        <v>20</v>
+      </c>
+      <c r="I31" s="10">
+        <v>0</v>
+      </c>
+      <c r="J31" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31" s="19">
+        <v>46069</v>
+      </c>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O31" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q31" s="16" t="str">
+        <f>HYPERLINK("[Icaffe_Export Sea_Operaton Test Cases.xlsx]OtherInvoice_Print!A1","Go to  OtherInvoice_Print")</f>
+        <v>Go to  OtherInvoice_Print</v>
+      </c>
+      <c r="R31" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="S31" s="2"/>
+    </row>
+    <row r="32" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>31</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="10">
+        <v>2</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10">
+        <v>2</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K32" s="19">
+        <v>46069</v>
+      </c>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O32" s="50"/>
+      <c r="P32" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q32" s="16" t="str">
+        <f>HYPERLINK("[Icaffe_Export Sea_Operaton Test Cases.xlsx]OtherInvoice_Print!A1","Go to  OtherInvoice_Print")</f>
+        <v>Go to  OtherInvoice_Print</v>
+      </c>
+      <c r="R32" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="S32" s="2"/>
+    </row>
+    <row r="33" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>32</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="10">
+        <v>93</v>
+      </c>
+      <c r="E33" s="10">
+        <v>78</v>
+      </c>
+      <c r="F33" s="10">
+        <v>15</v>
+      </c>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10">
+        <v>15</v>
+      </c>
+      <c r="I33" s="10">
+        <v>0</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K33" s="19">
+        <v>46070</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="O33" s="2"/>
+      <c r="P33" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q33" s="16" t="str">
+        <f>HYPERLINK("[Icaffe_Export Sea_Operaton Test Cases.xlsx]Consultancy_Invoice!A1","Go to  Consultancy_Invoice")</f>
+        <v>Go to  Consultancy_Invoice</v>
+      </c>
+      <c r="R33" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="S33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>